<commit_message>
FIX loi giao dien
</commit_message>
<xml_diff>
--- a/DS_SINH_VIEN.xlsx
+++ b/DS_SINH_VIEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAI HOC\Code BTL\Student-Management-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BE2D7E-1998-47B7-8951-D6609FF5F89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C27FDCF-F13D-4977-8F08-025461E36307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8503A00F-5CB8-4925-A8BA-6B20D2876729}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="154">
   <si>
     <t>ma_sinh_vien</t>
   </si>
@@ -86,16 +86,418 @@
     <t>B22DCVT007</t>
   </si>
   <si>
-    <t>Dương Thị Hông Anh</t>
-  </si>
-  <si>
-    <t>Honganh@ptit.edu.vn</t>
-  </si>
-  <si>
     <t>Hà Đông , Hà Nội</t>
   </si>
   <si>
-    <t>Trungnghia@ptit.edu.vn</t>
+    <t>B22DCVT015</t>
+  </si>
+  <si>
+    <t>B22DCVT047</t>
+  </si>
+  <si>
+    <t>B22DCVT055</t>
+  </si>
+  <si>
+    <t>B22DCVT079</t>
+  </si>
+  <si>
+    <t>B22DCVT087</t>
+  </si>
+  <si>
+    <t>B22DCVT095</t>
+  </si>
+  <si>
+    <t>B22DCVT111</t>
+  </si>
+  <si>
+    <t>B21DCVT123</t>
+  </si>
+  <si>
+    <t>B22DCVT135</t>
+  </si>
+  <si>
+    <t>B22DCVT143</t>
+  </si>
+  <si>
+    <t>B22DCVT159</t>
+  </si>
+  <si>
+    <t>B22DCVT167</t>
+  </si>
+  <si>
+    <t>B22DCVT183</t>
+  </si>
+  <si>
+    <t>B22DCVT191</t>
+  </si>
+  <si>
+    <t>B22DCVT199</t>
+  </si>
+  <si>
+    <t>B22DCVT207</t>
+  </si>
+  <si>
+    <t>B22DCVT215</t>
+  </si>
+  <si>
+    <t>B22DCVT223</t>
+  </si>
+  <si>
+    <t>B22DCVT231</t>
+  </si>
+  <si>
+    <t>B22DCVT239</t>
+  </si>
+  <si>
+    <t>B22DCVT247</t>
+  </si>
+  <si>
+    <t>B22DCVT279</t>
+  </si>
+  <si>
+    <t>B22DCVT287</t>
+  </si>
+  <si>
+    <t>B22DCVT295</t>
+  </si>
+  <si>
+    <t>B22DCVT311</t>
+  </si>
+  <si>
+    <t>B22DCVT327</t>
+  </si>
+  <si>
+    <t>B22DCVT359</t>
+  </si>
+  <si>
+    <t>B22DCVT367</t>
+  </si>
+  <si>
+    <t>B22DCVT399</t>
+  </si>
+  <si>
+    <t>B22DCVT407</t>
+  </si>
+  <si>
+    <t>B22DCVT423</t>
+  </si>
+  <si>
+    <t>B22DCVT439</t>
+  </si>
+  <si>
+    <t>B22DCVT511</t>
+  </si>
+  <si>
+    <t>B22DCVT535</t>
+  </si>
+  <si>
+    <t>B22DCVT559</t>
+  </si>
+  <si>
+    <t>B22DCVT567</t>
+  </si>
+  <si>
+    <t>B22DCVT575</t>
+  </si>
+  <si>
+    <t>B22DCVT479</t>
+  </si>
+  <si>
+    <t>B22DCVT495</t>
+  </si>
+  <si>
+    <t>B22DCVT503</t>
+  </si>
+  <si>
+    <t>B22DCVT583</t>
+  </si>
+  <si>
+    <t>B22DCVT591</t>
+  </si>
+  <si>
+    <t>B22DCVT424</t>
+  </si>
+  <si>
+    <t>B20DCVT210</t>
+  </si>
+  <si>
+    <t>Dương Thị Hồng Anh</t>
+  </si>
+  <si>
+    <t>Hoàng Quốc Anh</t>
+  </si>
+  <si>
+    <t>Bùi Gia Bảo</t>
+  </si>
+  <si>
+    <t>Kiều Quỳnh Biển</t>
+  </si>
+  <si>
+    <t>Nguyễn Văn Chiến</t>
+  </si>
+  <si>
+    <t>Đặng Tấn Dũng</t>
+  </si>
+  <si>
+    <t>Vũ Quang Dũng</t>
+  </si>
+  <si>
+    <t>Lê Đình Dương</t>
+  </si>
+  <si>
+    <t>Phan Văn Đạt</t>
+  </si>
+  <si>
+    <t>Vũ Tiến Đạt</t>
+  </si>
+  <si>
+    <t>Cổ Hữu Điềm</t>
+  </si>
+  <si>
+    <t>Nguyễn Trung Đức</t>
+  </si>
+  <si>
+    <t>Trần Trường Giang</t>
+  </si>
+  <si>
+    <t>Lê Thị Thúy Hằng</t>
+  </si>
+  <si>
+    <t>Hà Quang Hiếu</t>
+  </si>
+  <si>
+    <t>Đào Công Hòa</t>
+  </si>
+  <si>
+    <t>Ngô Trí Hoàng</t>
+  </si>
+  <si>
+    <t>Phạm Huy Hùng</t>
+  </si>
+  <si>
+    <t>Đào Huy Hùng</t>
+  </si>
+  <si>
+    <t>Bùi Quang Huy</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoàng Lê Huy</t>
+  </si>
+  <si>
+    <t>Trần Văn Huy</t>
+  </si>
+  <si>
+    <t>Dương Thế Khanh</t>
+  </si>
+  <si>
+    <t>Trần Quốc Khánh</t>
+  </si>
+  <si>
+    <t>Nông Đình Khôi</t>
+  </si>
+  <si>
+    <t>Vũ Đức Linh</t>
+  </si>
+  <si>
+    <t>Đỗ Tiến Mạnh</t>
+  </si>
+  <si>
+    <t>Nguyễn Hoài Nam</t>
+  </si>
+  <si>
+    <t>Nguyễn Viết Thiên Nam</t>
+  </si>
+  <si>
+    <t>Nguyễn Tuấn Phong</t>
+  </si>
+  <si>
+    <t>Lê Tài Phước</t>
+  </si>
+  <si>
+    <t>Nguyễn Hồng Quân</t>
+  </si>
+  <si>
+    <t>Lê Hữu Sơn</t>
+  </si>
+  <si>
+    <t>Đinh Tuấn Thành</t>
+  </si>
+  <si>
+    <t>Bùi Phú Thịnh</t>
+  </si>
+  <si>
+    <t>Nguyễn Trọng Triệu</t>
+  </si>
+  <si>
+    <t>Vương Hữu Trương</t>
+  </si>
+  <si>
+    <t>Phùng Xuân Trường</t>
+  </si>
+  <si>
+    <t>Đinh Văn Tuấn</t>
+  </si>
+  <si>
+    <t>Hoàng Thanh Tùng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Quang Tuyền </t>
+  </si>
+  <si>
+    <t>Nguyễn Thành Vinh</t>
+  </si>
+  <si>
+    <t>Lê Hải Vũ</t>
+  </si>
+  <si>
+    <t>Trần Thế Vương</t>
+  </si>
+  <si>
+    <t>Đỗ Quang Khải</t>
+  </si>
+  <si>
+    <t>D21VTVT</t>
+  </si>
+  <si>
+    <t>D20VTVT</t>
+  </si>
+  <si>
+    <t>AnhDTH.B22VT007@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>AnhHQ.B22VT015@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>BaoBG.B22VT047@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>BienKQ.B22VT055@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>ChienNV.B22VT079@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DungDT.B22VT087@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DungVQ.B22VT095@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DuongLD.B22VT111@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DatPV.B21VT123@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DatVT.B22VT135@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DiemCH.B22VT143@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>DucNT.B22VT159@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>GiangTT.B22VT167@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HangLTT.B22VT183@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HieuHQ.B22VT191@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HoaDC.B22VT199@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HoangNT.B22VT207@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HoangPH.B22VT215@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HungDH.B22VT223@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HuyBQ.B22VT231@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HuyNHL.B22VT239@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>HuyTV.B22VT247@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>KhanhDT.B22VT279@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>KhanhTQ.B22VT287@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>KhoiND.B22VT295@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>LinhVD.B22VT311@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>ManhDT.B22VT327@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>NamNH.B22VT359@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>NamNVT.B22VT367@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>NghiaTT.B22VT391@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>PhongNT.B22VT399@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>PhuocLT.B22VT407@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>QuanNH.B22VT423@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>SonLH.B22VT439@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>ThanhDT.B22VT511@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>ThinhBP.B22VT535@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>TrieuNT.B22VT559@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>TruongVH.B22VT567@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>TruongPX.B22VT575@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>TuanDV.B22VT479@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>TungHT.B22VT495@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>TuyenNQ.B22VT503@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>VinhNT.B22VT583@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>VuLH.B22VT591@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>VuongTT.B20VT424@stu.ptit.edu.vn</t>
+  </si>
+  <si>
+    <t>KhaiDQ.B20VT210@stu.ptit.edu.vn</t>
   </si>
 </sst>
 </file>
@@ -105,7 +507,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,16 +562,27 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -499,13 +912,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BEF1187-E5C8-4EE6-B5A1-3D770EB841B5}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="19.109375" customWidth="1"/>
     <col min="2" max="2" width="19.77734375" customWidth="1"/>
@@ -517,7 +930,7 @@
     <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -546,12 +959,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>61</v>
       </c>
       <c r="C2">
         <v>12345</v>
@@ -559,8 +972,8 @@
       <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
+      <c r="E2" t="s">
+        <v>108</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -571,56 +984,1063 @@
       <c r="H2" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>37993</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3">
+        <v>12345</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="C3">
-        <v>12345</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I8" s="4"/>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4">
+        <v>12345</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>12345</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>12345</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7">
+        <v>12345</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8">
+        <v>12345</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="3"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9">
+        <v>12345</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10">
+        <v>12345</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="G10" t="s">
+        <v>106</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11">
+        <v>12345</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12">
+        <v>12345</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13">
+        <v>12345</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14">
+        <v>12345</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>120</v>
+      </c>
+      <c r="G14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15">
+        <v>12345</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16">
+        <v>12345</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17">
+        <v>12345</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18">
+        <v>12345</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" t="s">
+        <v>124</v>
+      </c>
+      <c r="G18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19">
+        <v>12345</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>125</v>
+      </c>
+      <c r="G19" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20">
+        <v>12345</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21">
+        <v>12345</v>
+      </c>
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>127</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22">
+        <v>12345</v>
+      </c>
+      <c r="D22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" t="s">
+        <v>128</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23">
+        <v>12345</v>
+      </c>
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>129</v>
+      </c>
+      <c r="G23" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24">
+        <v>12345</v>
+      </c>
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25">
+        <v>12345</v>
+      </c>
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G25" t="s">
+        <v>13</v>
+      </c>
+      <c r="H25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26">
+        <v>12345</v>
+      </c>
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27">
+        <v>12345</v>
+      </c>
+      <c r="D27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>133</v>
+      </c>
+      <c r="G27" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28">
+        <v>12345</v>
+      </c>
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29">
+        <v>12345</v>
+      </c>
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30">
+        <v>12345</v>
+      </c>
+      <c r="D30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>12345</v>
+      </c>
+      <c r="D31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>137</v>
+      </c>
+      <c r="G31" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C32">
+        <v>12345</v>
+      </c>
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>138</v>
+      </c>
+      <c r="G32" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33">
+        <v>12345</v>
+      </c>
+      <c r="D33" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" t="s">
+        <v>139</v>
+      </c>
+      <c r="G33" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C34">
+        <v>12345</v>
+      </c>
+      <c r="D34" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35">
+        <v>12345</v>
+      </c>
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>141</v>
+      </c>
+      <c r="G35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36">
+        <v>12345</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>142</v>
+      </c>
+      <c r="G36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" t="s">
+        <v>95</v>
+      </c>
+      <c r="C37">
+        <v>12345</v>
+      </c>
+      <c r="D37" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" t="s">
+        <v>143</v>
+      </c>
+      <c r="G37" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" t="s">
+        <v>96</v>
+      </c>
+      <c r="C38">
+        <v>12345</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" t="s">
+        <v>52</v>
+      </c>
+      <c r="B39" t="s">
+        <v>97</v>
+      </c>
+      <c r="C39">
+        <v>12345</v>
+      </c>
+      <c r="D39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" t="s">
+        <v>145</v>
+      </c>
+      <c r="G39" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" t="s">
+        <v>98</v>
+      </c>
+      <c r="C40">
+        <v>12345</v>
+      </c>
+      <c r="D40" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" t="s">
+        <v>146</v>
+      </c>
+      <c r="G40" t="s">
+        <v>13</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41">
+        <v>12345</v>
+      </c>
+      <c r="D41" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" t="s">
+        <v>147</v>
+      </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
+      <c r="H41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>100</v>
+      </c>
+      <c r="C42">
+        <v>12345</v>
+      </c>
+      <c r="D42" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" t="s">
+        <v>148</v>
+      </c>
+      <c r="G42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H42" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43">
+        <v>12345</v>
+      </c>
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>149</v>
+      </c>
+      <c r="G43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H43" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" t="s">
+        <v>57</v>
+      </c>
+      <c r="B44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C44">
+        <v>12345</v>
+      </c>
+      <c r="D44" t="s">
+        <v>11</v>
+      </c>
+      <c r="E44" t="s">
+        <v>150</v>
+      </c>
+      <c r="G44" t="s">
+        <v>13</v>
+      </c>
+      <c r="H44" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" t="s">
+        <v>58</v>
+      </c>
+      <c r="B45" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45">
+        <v>12345</v>
+      </c>
+      <c r="D45" t="s">
+        <v>11</v>
+      </c>
+      <c r="E45" t="s">
+        <v>151</v>
+      </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
+      <c r="H45" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46">
+        <v>12345</v>
+      </c>
+      <c r="D46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G46" t="s">
+        <v>107</v>
+      </c>
+      <c r="H46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47">
+        <v>12345</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G47" t="s">
+        <v>107</v>
+      </c>
+      <c r="H47" t="s">
+        <v>14</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="F2:F47">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Hà đông ,Hà Nội">
+      <formula>NOT(ISERROR(SEARCH("Hà đông ,Hà Nội",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{6008BF81-1D79-4D30-BCD3-A61CE0A7970D}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{36A4620B-97E2-49DC-A078-8B68B29F9EA0}"/>
+    <hyperlink ref="E46" r:id="rId1" xr:uid="{0C307053-9F6A-4979-8CEC-99B226ACCFF3}"/>
+    <hyperlink ref="E47" r:id="rId2" xr:uid="{BCB4FD93-1119-4340-9FB4-D6F4D34EEF0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
update fix loi giao dien
</commit_message>
<xml_diff>
--- a/DS_SINH_VIEN.xlsx
+++ b/DS_SINH_VIEN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DAI HOC\Code BTL\Student-Management-Web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C27FDCF-F13D-4977-8F08-025461E36307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52E5E24-CAD3-4D16-BBD3-ABB35E5685C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8503A00F-5CB8-4925-A8BA-6B20D2876729}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="152">
   <si>
     <t>ma_sinh_vien</t>
   </si>
@@ -74,9 +74,6 @@
     <t>SINHVIEN</t>
   </si>
   <si>
-    <t>Hà đông ,Hà Nội</t>
-  </si>
-  <si>
     <t>D22CQVT07-B</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
   </si>
   <si>
     <t>B22DCVT007</t>
-  </si>
-  <si>
-    <t>Hà Đông , Hà Nội</t>
   </si>
   <si>
     <t>B22DCVT015</t>
@@ -915,7 +909,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -924,9 +918,9 @@
     <col min="2" max="2" width="19.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" customWidth="1"/>
-    <col min="6" max="6" width="18.21875" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="38.21875" customWidth="1"/>
+    <col min="6" max="6" width="48.21875" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
     <col min="9" max="9" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -961,10 +955,10 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>12345</v>
@@ -973,16 +967,13 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I2" s="2">
         <v>37993</v>
@@ -990,10 +981,10 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C3">
         <v>12345</v>
@@ -1002,25 +993,22 @@
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
+        <v>107</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C4">
         <v>12345</v>
@@ -1029,22 +1017,22 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C5">
         <v>12345</v>
@@ -1053,22 +1041,22 @@
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6">
         <v>12345</v>
@@ -1077,22 +1065,22 @@
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C7">
         <v>12345</v>
@@ -1101,22 +1089,22 @@
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C8">
         <v>12345</v>
@@ -1125,22 +1113,22 @@
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C9">
         <v>12345</v>
@@ -1149,21 +1137,21 @@
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>12345</v>
@@ -1172,21 +1160,21 @@
         <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C11">
         <v>12345</v>
@@ -1195,21 +1183,21 @@
         <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C12">
         <v>12345</v>
@@ -1218,21 +1206,21 @@
         <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>12345</v>
@@ -1241,21 +1229,21 @@
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14">
         <v>12345</v>
@@ -1264,21 +1252,21 @@
         <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15">
         <v>12345</v>
@@ -1287,21 +1275,21 @@
         <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C16">
         <v>12345</v>
@@ -1310,21 +1298,21 @@
         <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C17">
         <v>12345</v>
@@ -1333,21 +1321,21 @@
         <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C18">
         <v>12345</v>
@@ -1356,21 +1344,21 @@
         <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C19">
         <v>12345</v>
@@ -1379,21 +1367,21 @@
         <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C20">
         <v>12345</v>
@@ -1402,21 +1390,21 @@
         <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21">
         <v>12345</v>
@@ -1425,21 +1413,21 @@
         <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22">
         <v>12345</v>
@@ -1448,21 +1436,21 @@
         <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23">
         <v>12345</v>
@@ -1471,21 +1459,21 @@
         <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G23" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C24">
         <v>12345</v>
@@ -1494,21 +1482,21 @@
         <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C25">
         <v>12345</v>
@@ -1517,21 +1505,21 @@
         <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G25" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H25" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C26">
         <v>12345</v>
@@ -1540,21 +1528,21 @@
         <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C27">
         <v>12345</v>
@@ -1563,21 +1551,21 @@
         <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G27" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C28">
         <v>12345</v>
@@ -1586,21 +1574,21 @@
         <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C29">
         <v>12345</v>
@@ -1609,21 +1597,21 @@
         <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C30">
         <v>12345</v>
@@ -1632,13 +1620,13 @@
         <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G30" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H30" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1655,21 +1643,21 @@
         <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C32">
         <v>12345</v>
@@ -1678,21 +1666,21 @@
         <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H32" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C33">
         <v>12345</v>
@@ -1701,21 +1689,21 @@
         <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C34">
         <v>12345</v>
@@ -1724,21 +1712,21 @@
         <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:8">
       <c r="A35" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C35">
         <v>12345</v>
@@ -1747,21 +1735,21 @@
         <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C36">
         <v>12345</v>
@@ -1770,21 +1758,21 @@
         <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:8">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C37">
         <v>12345</v>
@@ -1793,21 +1781,21 @@
         <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C38">
         <v>12345</v>
@@ -1816,21 +1804,21 @@
         <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H38" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:8">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B39" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39">
         <v>12345</v>
@@ -1839,21 +1827,21 @@
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G39" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H39" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40">
         <v>12345</v>
@@ -1862,21 +1850,21 @@
         <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G40" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H40" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B41" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41">
         <v>12345</v>
@@ -1885,21 +1873,21 @@
         <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G41" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H41" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>12345</v>
@@ -1908,21 +1896,21 @@
         <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G42" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43">
         <v>12345</v>
@@ -1931,21 +1919,21 @@
         <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <v>12345</v>
@@ -1954,21 +1942,21 @@
         <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B45" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C45">
         <v>12345</v>
@@ -1977,21 +1965,21 @@
         <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G45" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B46" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C46">
         <v>12345</v>
@@ -2000,36 +1988,36 @@
         <v>11</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G46" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:8">
       <c r="A47" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47">
+        <v>12345</v>
+      </c>
+      <c r="D47" t="s">
+        <v>11</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G47" t="s">
         <v>105</v>
       </c>
-      <c r="C47">
-        <v>12345</v>
-      </c>
-      <c r="D47" t="s">
-        <v>11</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="G47" t="s">
-        <v>107</v>
-      </c>
       <c r="H47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>